<commit_message>
added test files for excel and pytest for excel.
</commit_message>
<xml_diff>
--- a/tests/data/cars.xlsx
+++ b/tests/data/cars.xlsx
@@ -113,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -128,9 +128,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -594,54 +591,56 @@
     </row>
     <row r="5">
       <c r="A5" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>110</v>
+      </c>
+      <c r="E5" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13" t="n">
+        <v>2.7475</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>0.1803122292025695</v>
+      </c>
+      <c r="H5" s="9" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B6" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="n">
+      <c r="C6" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D6" s="13" t="n">
         <v>83.33333333333333</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E6" s="13" t="n">
         <v>18.50225211517056</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F6" s="13" t="n">
         <v>2.886666666666667</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G6" s="13" t="n">
         <v>0.4911551010967242</v>
       </c>
-      <c r="H5" s="9" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="14" t="n">
+      <c r="H6" s="9" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="13" t="n">
-        <v>110</v>
-      </c>
-      <c r="E6" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="13" t="n">
-        <v>2.7475</v>
-      </c>
-      <c r="G6" s="13" t="n">
-        <v>0.1803122292025695</v>
-      </c>
-      <c r="H6" s="9" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="n"/>
       <c r="B7" s="12" t="n">
         <v>1</v>
       </c>
@@ -687,25 +686,24 @@
       <c r="H8" s="9" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="inlineStr">
+      <c r="A9" s="14" t="inlineStr">
         <is>
           <t>Data from the infamous mtcars data set.</t>
         </is>
       </c>
-      <c r="B9" s="16" t="n"/>
-      <c r="C9" s="16" t="n"/>
-      <c r="D9" s="16" t="n"/>
-      <c r="E9" s="16" t="n"/>
-      <c r="F9" s="16" t="n"/>
-      <c r="G9" s="16" t="n"/>
+      <c r="B9" s="15" t="n"/>
+      <c r="C9" s="15" t="n"/>
+      <c r="D9" s="15" t="n"/>
+      <c r="E9" s="15" t="n"/>
+      <c r="F9" s="15" t="n"/>
+      <c r="G9" s="15" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A6:A7"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added sorting to the test files to test merging of columns
</commit_message>
<xml_diff>
--- a/tests/data/cars.xlsx
+++ b/tests/data/cars.xlsx
@@ -113,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -128,6 +128,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -591,56 +594,54 @@
     </row>
     <row r="5">
       <c r="A5" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>83.33333333333333</v>
+      </c>
+      <c r="E5" s="13" t="n">
+        <v>18.50225211517056</v>
+      </c>
+      <c r="F5" s="13" t="n">
+        <v>2.886666666666667</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>0.4911551010967242</v>
+      </c>
+      <c r="H5" s="9" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B6" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="11" t="n">
+      <c r="C6" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D6" s="13" t="n">
         <v>110</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E6" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F6" s="13" t="n">
         <v>2.7475</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G6" s="13" t="n">
         <v>0.1803122292025695</v>
       </c>
-      <c r="H5" s="9" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="13" t="n">
-        <v>83.33333333333333</v>
-      </c>
-      <c r="E6" s="13" t="n">
-        <v>18.50225211517056</v>
-      </c>
-      <c r="F6" s="13" t="n">
-        <v>2.886666666666667</v>
-      </c>
-      <c r="G6" s="13" t="n">
-        <v>0.4911551010967242</v>
-      </c>
       <c r="H6" s="9" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="n">
-        <v>6</v>
-      </c>
+      <c r="A7" s="9" t="n"/>
       <c r="B7" s="12" t="n">
         <v>1</v>
       </c>
@@ -686,24 +687,25 @@
       <c r="H8" s="9" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="inlineStr">
+      <c r="A9" s="15" t="inlineStr">
         <is>
           <t>Data from the infamous mtcars data set.</t>
         </is>
       </c>
-      <c r="B9" s="15" t="n"/>
-      <c r="C9" s="15" t="n"/>
-      <c r="D9" s="15" t="n"/>
-      <c r="E9" s="15" t="n"/>
-      <c r="F9" s="15" t="n"/>
-      <c r="G9" s="15" t="n"/>
+      <c r="B9" s="16" t="n"/>
+      <c r="C9" s="16" t="n"/>
+      <c r="D9" s="16" t="n"/>
+      <c r="E9" s="16" t="n"/>
+      <c r="F9" s="16" t="n"/>
+      <c r="G9" s="16" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added mtcars data set
</commit_message>
<xml_diff>
--- a/tests/data/cars.xlsx
+++ b/tests/data/cars.xlsx
@@ -125,12 +125,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,116 +597,135 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="n">
+      <c r="D5" s="14" t="n">
+        <v>91</v>
+      </c>
+      <c r="E5" s="14" t="n"/>
+      <c r="F5" s="14" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="G5" s="14" t="n"/>
+      <c r="H5" s="9" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="n"/>
+      <c r="B6" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <v>21.87235698318771</v>
+      </c>
+      <c r="F6" s="14" t="n">
+        <v>2.3003</v>
+      </c>
+      <c r="G6" s="14" t="n">
+        <v>0.5982073312080948</v>
+      </c>
+      <c r="H6" s="9" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="13" t="n">
-        <v>83.33333333333333</v>
-      </c>
-      <c r="E5" s="13" t="n">
-        <v>18.50225211517056</v>
-      </c>
-      <c r="F5" s="13" t="n">
-        <v>2.886666666666667</v>
-      </c>
-      <c r="G5" s="13" t="n">
-        <v>0.4911551010967242</v>
-      </c>
-      <c r="H5" s="9" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="14" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" s="12" t="n">
+      <c r="D7" s="14" t="n">
+        <v>131.6666666666667</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <v>37.52776749732568</v>
+      </c>
+      <c r="F7" s="14" t="n">
+        <v>2.755</v>
+      </c>
+      <c r="G7" s="14" t="n">
+        <v>0.1281600561797629</v>
+      </c>
+      <c r="H7" s="9" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="n"/>
+      <c r="B8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="14" t="n">
+        <v>115.25</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <v>9.178779875342908</v>
+      </c>
+      <c r="F8" s="14" t="n">
+        <v>3.38875</v>
+      </c>
+      <c r="G8" s="14" t="n">
+        <v>0.1162163929916946</v>
+      </c>
+      <c r="H8" s="9" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="13" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="13" t="n">
-        <v>110</v>
-      </c>
-      <c r="E6" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="13" t="n">
-        <v>2.7475</v>
-      </c>
-      <c r="G6" s="13" t="n">
-        <v>0.1803122292025695</v>
-      </c>
-      <c r="H6" s="9" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="n"/>
-      <c r="B7" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="13" t="n">
-        <v>112.6666666666667</v>
-      </c>
-      <c r="E7" s="13" t="n">
-        <v>9.291573243177568</v>
-      </c>
-      <c r="F7" s="13" t="n">
-        <v>3.371666666666667</v>
-      </c>
-      <c r="G7" s="13" t="n">
-        <v>0.1360453355809502</v>
-      </c>
-      <c r="H7" s="9" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B8" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="13" t="n">
-        <v>210</v>
-      </c>
-      <c r="E8" s="13" t="n">
-        <v>49.49747468305833</v>
-      </c>
-      <c r="F8" s="13" t="n">
-        <v>3.505</v>
-      </c>
-      <c r="G8" s="13" t="n">
-        <v>0.0919238815542511</v>
-      </c>
-      <c r="H8" s="9" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="15" t="inlineStr">
+      <c r="C9" s="13" t="n">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>209.2142857142857</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <v>50.97688551827051</v>
+      </c>
+      <c r="F9" s="14" t="n">
+        <v>3.999214285714287</v>
+      </c>
+      <c r="G9" s="14" t="n">
+        <v>0.7594047444769265</v>
+      </c>
+      <c r="H9" s="9" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="15" t="inlineStr">
         <is>
           <t>Data from the infamous mtcars data set.</t>
         </is>
       </c>
-      <c r="B9" s="16" t="n"/>
-      <c r="C9" s="16" t="n"/>
-      <c r="D9" s="16" t="n"/>
-      <c r="E9" s="16" t="n"/>
-      <c r="F9" s="16" t="n"/>
-      <c r="G9" s="16" t="n"/>
+      <c r="B10" s="16" t="n"/>
+      <c r="C10" s="16" t="n"/>
+      <c r="D10" s="16" t="n"/>
+      <c r="E10" s="16" t="n"/>
+      <c r="F10" s="16" t="n"/>
+      <c r="G10" s="16" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A6:A7"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>